<commit_message>
LDAP Client Linux finish
</commit_message>
<xml_diff>
--- a/Arbeitsaufteilung.xlsx
+++ b/Arbeitsaufteilung.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adin Karic\Desktop\LDAP\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Aufgaben</t>
   </si>
@@ -120,13 +115,16 @@
   </si>
   <si>
     <t>Kopec, Ernhofer</t>
+  </si>
+  <si>
+    <t>180min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -197,15 +195,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -558,17 +556,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="103.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.625" customWidth="1"/>
-    <col min="4" max="4" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.875" customWidth="1"/>
-    <col min="6" max="6" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="103.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6">
@@ -730,6 +728,15 @@
     <row r="30" spans="2:6">
       <c r="B30" t="s">
         <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="2">
+        <v>42069</v>
+      </c>
+      <c r="E30" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>